<commit_message>
Making some test ROMs work
</commit_message>
<xml_diff>
--- a/ROM Progess.xlsx
+++ b/ROM Progess.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t>DEMOS</t>
   </si>
@@ -127,13 +127,19 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Ordre des lettres semble quasi aléatore</t>
+  </si>
+  <si>
+    <t>Image statique</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +159,12 @@
       <i/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -447,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -481,6 +493,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -776,21 +790,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:I34"/>
+  <dimension ref="B1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="46" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:9" ht="15.75">
+    <row r="1" spans="2:7" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:7" ht="15.75">
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
         <v>30</v>
@@ -799,14 +814,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="26.25">
+    <row r="3" spans="2:7" ht="26.25">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="2:9" ht="15.75" thickBot="1">
+    <row r="4" spans="2:7" ht="15.75" thickBot="1">
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
@@ -815,7 +830,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="15.75" thickBot="1">
+    <row r="5" spans="2:7" ht="15.75" thickBot="1">
       <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
@@ -823,12 +838,12 @@
       <c r="D5" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="F5" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="17"/>
-    </row>
-    <row r="6" spans="2:9">
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="2:7">
       <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
@@ -836,12 +851,12 @@
       <c r="D6" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="F6" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="21"/>
-    </row>
-    <row r="7" spans="2:9">
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="2:7">
       <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
@@ -849,25 +864,25 @@
       <c r="D7" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="19"/>
-    </row>
-    <row r="8" spans="2:9" ht="15.75" thickBot="1">
+      <c r="G7" s="19"/>
+    </row>
+    <row r="8" spans="2:7" ht="15.75" thickBot="1">
       <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="20"/>
-    </row>
-    <row r="9" spans="2:9">
+      <c r="G8" s="20"/>
+    </row>
+    <row r="9" spans="2:7">
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
@@ -876,7 +891,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:7">
       <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
@@ -885,7 +900,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:7">
       <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
@@ -894,7 +909,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:7">
       <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
@@ -903,7 +918,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:7">
       <c r="B13" s="8" t="s">
         <v>10</v>
       </c>
@@ -912,7 +927,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:7">
       <c r="B14" s="8" t="s">
         <v>11</v>
       </c>
@@ -921,7 +936,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:7">
       <c r="B15" s="8" t="s">
         <v>12</v>
       </c>
@@ -930,7 +945,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:7">
       <c r="B16" s="8" t="s">
         <v>13</v>
       </c>
@@ -1030,7 +1045,7 @@
       <c r="B28" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="25"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="23" t="s">
         <v>36</v>
       </c>
@@ -1048,9 +1063,9 @@
       <c r="B30" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="23" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="2:4">
@@ -1066,7 +1081,7 @@
       <c r="B32" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="2"/>
+      <c r="C32" s="25"/>
       <c r="D32" s="23" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Up to 10 working ROMs
</commit_message>
<xml_diff>
--- a/ROM Progess.xlsx
+++ b/ROM Progess.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t>DEMOS</t>
   </si>
@@ -129,10 +129,28 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Ordre des lettres semble quasi aléatore</t>
-  </si>
-  <si>
-    <t>Image statique</t>
+    <t>Hyper-espace (comme dans Star Wars)</t>
+  </si>
+  <si>
+    <t>Palette veut se cacher + mauvaises couleurs</t>
+  </si>
+  <si>
+    <t>Problèmes au niveau des contrôles + ne détecte pas les collisions</t>
+  </si>
+  <si>
+    <t>Problème</t>
+  </si>
+  <si>
+    <t>Le background devrait être blanc à la fin</t>
+  </si>
+  <si>
+    <t>Écran noir + Unknown opcode</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>Pacman</t>
   </si>
 </sst>
 </file>
@@ -170,7 +188,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,8 +219,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -441,25 +465,58 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -481,12 +538,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -495,7 +549,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -790,17 +859,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:G34"/>
+  <dimension ref="B1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="46" customWidth="1"/>
+    <col min="4" max="4" width="58.7109375" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -826,7 +895,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="20" t="s">
         <v>36</v>
       </c>
     </row>
@@ -834,78 +903,82 @@
       <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="22" t="s">
+      <c r="C5" s="22"/>
+      <c r="D5" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="17"/>
+      <c r="G5" s="30"/>
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="13" t="s">
+      <c r="C6" s="22"/>
+      <c r="D6" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="21"/>
+      <c r="G6" s="26"/>
     </row>
     <row r="7" spans="2:7">
       <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="23" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="20" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="19"/>
-    </row>
-    <row r="8" spans="2:7" ht="15.75" thickBot="1">
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="2:7">
       <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="20"/>
-    </row>
-    <row r="9" spans="2:7">
+      <c r="C8" s="22"/>
+      <c r="D8" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="28"/>
+    </row>
+    <row r="9" spans="2:7" ht="15.75" thickBot="1">
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="23" t="s">
-        <v>36</v>
-      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="23" t="s">
-        <v>36</v>
+      <c r="C10" s="25"/>
+      <c r="D10" s="20" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="23" t="s">
+      <c r="C11" s="22"/>
+      <c r="D11" s="20" t="s">
         <v>36</v>
       </c>
     </row>
@@ -914,7 +987,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="20" t="s">
         <v>36</v>
       </c>
     </row>
@@ -922,17 +995,17 @@
       <c r="B13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="23" t="s">
-        <v>36</v>
+      <c r="C13" s="25"/>
+      <c r="D13" s="20" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="2:7">
       <c r="B14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="23" t="s">
+      <c r="C14" s="22"/>
+      <c r="D14" s="20" t="s">
         <v>36</v>
       </c>
     </row>
@@ -940,8 +1013,8 @@
       <c r="B15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="23" t="s">
+      <c r="C15" s="22"/>
+      <c r="D15" s="20" t="s">
         <v>36</v>
       </c>
     </row>
@@ -949,162 +1022,182 @@
       <c r="B16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="24"/>
-    </row>
-    <row r="18" spans="2:4" ht="27" thickBot="1">
-      <c r="B18" s="15" t="s">
+      <c r="C16" s="22"/>
+      <c r="D16" s="20"/>
+    </row>
+    <row r="17" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B18" s="31"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="33"/>
+      <c r="F18" s="24"/>
+    </row>
+    <row r="19" spans="2:6" ht="27" thickBot="1">
+      <c r="B19" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="23"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="13" t="s">
+      <c r="C19" s="16"/>
+      <c r="D19" s="20"/>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="8" t="s">
+      <c r="C20" s="14"/>
+      <c r="D20" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="8" t="s">
+      <c r="C21" s="2"/>
+      <c r="D21" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="2"/>
+      <c r="D22" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="8" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="8" t="s">
+      <c r="C25" s="2"/>
+      <c r="D25" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B25" s="11"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="24"/>
-    </row>
-    <row r="26" spans="2:4" ht="27" thickBot="1">
-      <c r="B26" s="15" t="s">
+      <c r="C26" s="2"/>
+      <c r="D26" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B27" s="11"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="21"/>
+    </row>
+    <row r="28" spans="2:6" ht="27" thickBot="1">
+      <c r="B28" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="23"/>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" s="13" t="s">
+      <c r="C28" s="17"/>
+      <c r="D28" s="20"/>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="8" t="s">
+      <c r="C29" s="14"/>
+      <c r="D29" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="8" t="s">
+      <c r="C30" s="23"/>
+      <c r="D30" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30" s="8" t="s">
+      <c r="C31" s="25"/>
+      <c r="D31" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="27"/>
-      <c r="D30" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4">
-      <c r="B31" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="23" t="s">
+      <c r="C32" s="22"/>
+      <c r="D32" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="22"/>
+      <c r="D33" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B34" s="9" t="s">
+      <c r="C35" s="25"/>
+      <c r="D35" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B36" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="23" t="s">
+      <c r="C36" s="10"/>
+      <c r="D36" s="20" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F5:G5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
More ROMs are now working
</commit_message>
<xml_diff>
--- a/ROM Progess.xlsx
+++ b/ROM Progess.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
   <si>
     <t>DEMOS</t>
   </si>
@@ -132,32 +132,56 @@
     <t>Hyper-espace (comme dans Star Wars)</t>
   </si>
   <si>
-    <t>Palette veut se cacher + mauvaises couleurs</t>
-  </si>
-  <si>
-    <t>Problèmes au niveau des contrôles + ne détecte pas les collisions</t>
-  </si>
-  <si>
     <t>Problème</t>
   </si>
   <si>
-    <t>Le background devrait être blanc à la fin</t>
-  </si>
-  <si>
-    <t>Écran noir + Unknown opcode</t>
-  </si>
-  <si>
     <t>water</t>
   </si>
   <si>
     <t>Pacman</t>
+  </si>
+  <si>
+    <t>Test de son</t>
+  </si>
+  <si>
+    <t>Unknown opcode</t>
+  </si>
+  <si>
+    <t>Écran blanc en fin de partie</t>
+  </si>
+  <si>
+    <t>alien</t>
+  </si>
+  <si>
+    <t>tetris</t>
+  </si>
+  <si>
+    <t>Écran noir</t>
+  </si>
+  <si>
+    <t>Écran rouge après 1ère mort</t>
+  </si>
+  <si>
+    <t>boing</t>
+  </si>
+  <si>
+    <t>dots</t>
+  </si>
+  <si>
+    <t>pikachu</t>
+  </si>
+  <si>
+    <t>xor</t>
+  </si>
+  <si>
+    <t>MegaManX16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +207,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -516,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -554,17 +585,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -859,17 +894,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:G36"/>
+  <dimension ref="B1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="58.7109375" customWidth="1"/>
+    <col min="4" max="4" width="65.7109375" customWidth="1"/>
+    <col min="5" max="5" width="3.5703125" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -896,7 +932,7 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="20" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="15.75" thickBot="1">
@@ -907,10 +943,10 @@
       <c r="D5" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="30"/>
+      <c r="G5" s="33"/>
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="8" t="s">
@@ -940,258 +976,327 @@
     </row>
     <row r="8" spans="2:7">
       <c r="B8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="22"/>
+        <v>48</v>
+      </c>
+      <c r="C8" s="2"/>
       <c r="D8" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="28"/>
-    </row>
-    <row r="9" spans="2:7" ht="15.75" thickBot="1">
+      <c r="F8" s="8"/>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="2:7">
       <c r="B9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="25"/>
+        <v>49</v>
+      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="19"/>
+        <v>36</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="25"/>
+        <v>5</v>
+      </c>
+      <c r="C10" s="22"/>
       <c r="D10" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7">
+        <v>36</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="28"/>
+    </row>
+    <row r="11" spans="2:7" ht="15.75" thickBot="1">
       <c r="B11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="22"/>
+        <v>6</v>
+      </c>
+      <c r="C11" s="34"/>
       <c r="D11" s="20" t="s">
         <v>36</v>
       </c>
+      <c r="F11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="C12" s="22"/>
       <c r="D12" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="25"/>
+        <v>8</v>
+      </c>
+      <c r="C13" s="22"/>
       <c r="D13" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:7">
       <c r="B14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="22"/>
+        <v>50</v>
+      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="22"/>
+        <v>9</v>
+      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="20" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:7">
       <c r="B16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="20"/>
-    </row>
-    <row r="17" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B17" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B18" s="31"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="33"/>
-      <c r="F18" s="24"/>
-    </row>
-    <row r="19" spans="2:6" ht="27" thickBot="1">
-      <c r="B19" s="15" t="s">
+      <c r="C19" s="22"/>
+      <c r="D19" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="37"/>
+      <c r="D20" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B21" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="31"/>
+      <c r="F22" s="24"/>
+    </row>
+    <row r="23" spans="2:6" ht="27" thickBot="1">
+      <c r="B23" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="20"/>
-    </row>
-    <row r="20" spans="2:6">
-      <c r="B20" s="13" t="s">
+      <c r="C23" s="16"/>
+      <c r="D23" s="20"/>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="35"/>
+      <c r="D24" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="B21" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="B22" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6">
-      <c r="B23" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6">
-      <c r="B24" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6">
-      <c r="B25" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="21"/>
-    </row>
-    <row r="28" spans="2:6" ht="27" thickBot="1">
-      <c r="B28" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="20"/>
+    <row r="27" spans="2:6">
+      <c r="B27" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="20" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="29" spans="2:6">
-      <c r="B29" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="14"/>
+      <c r="B29" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="25"/>
       <c r="D29" s="20" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="23"/>
+        <v>18</v>
+      </c>
+      <c r="C30" s="22"/>
       <c r="D30" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="25"/>
+        <v>19</v>
+      </c>
+      <c r="C31" s="22"/>
       <c r="D31" s="20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="22"/>
+        <v>20</v>
+      </c>
+      <c r="C32" s="25"/>
       <c r="D32" s="20" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="25"/>
+      <c r="D33" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B34" s="11"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="21"/>
+    </row>
+    <row r="35" spans="2:4" ht="27" thickBot="1">
+      <c r="B35" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="17"/>
+      <c r="D35" s="20"/>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="23"/>
+      <c r="D37" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="B38" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="22"/>
+      <c r="D39" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="B34" s="8" t="s">
+      <c r="C40" s="22"/>
+      <c r="D40" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4">
-      <c r="B35" s="8" t="s">
+      <c r="C41" s="22"/>
+      <c r="D41" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="B42" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="25"/>
-      <c r="D35" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B36" s="9" t="s">
+      <c r="C42" s="22"/>
+      <c r="D42" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B43" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="20" t="s">
-        <v>36</v>
+      <c r="C43" s="10"/>
+      <c r="D43" s="20" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixing + weekly report + doc update
</commit_message>
<xml_diff>
--- a/ROM Progess.xlsx
+++ b/ROM Progess.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
   <si>
     <t>DEMOS</t>
   </si>
@@ -138,9 +138,6 @@
     <t>water</t>
   </si>
   <si>
-    <t>Pacman</t>
-  </si>
-  <si>
     <t>Test de son</t>
   </si>
   <si>
@@ -156,25 +153,22 @@
     <t>tetris</t>
   </si>
   <si>
-    <t>Écran noir</t>
-  </si>
-  <si>
     <t>Écran rouge après 1ère mort</t>
   </si>
   <si>
     <t>boing</t>
   </si>
   <si>
-    <t>dots</t>
-  </si>
-  <si>
-    <t>pikachu</t>
-  </si>
-  <si>
     <t>xor</t>
   </si>
   <si>
     <t>MegaManX16</t>
+  </si>
+  <si>
+    <t>dots2</t>
+  </si>
+  <si>
+    <t>Point unique alors qu'on devrait voir une droite</t>
   </si>
 </sst>
 </file>
@@ -547,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -599,7 +593,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -894,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:G43"/>
+  <dimension ref="B1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -932,7 +927,7 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="15.75" thickBot="1">
@@ -976,25 +971,29 @@
     </row>
     <row r="8" spans="2:7">
       <c r="B8" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="C8" s="22"/>
       <c r="D8" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="18"/>
-    </row>
-    <row r="9" spans="2:7">
+      <c r="F8" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="28"/>
+    </row>
+    <row r="9" spans="2:7" ht="15.75" thickBot="1">
       <c r="B9" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="18"/>
+        <v>50</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="8" t="s">
@@ -1004,12 +1003,8 @@
       <c r="D10" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="28"/>
-    </row>
-    <row r="11" spans="2:7" ht="15.75" thickBot="1">
+    </row>
+    <row r="11" spans="2:7">
       <c r="B11" s="8" t="s">
         <v>6</v>
       </c>
@@ -1017,10 +1012,6 @@
       <c r="D11" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="8" t="s">
@@ -1042,34 +1033,34 @@
     </row>
     <row r="14" spans="2:7">
       <c r="B14" s="8" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="20" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="C15" s="25"/>
       <c r="D15" s="20" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:7">
       <c r="B16" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="25"/>
+        <v>11</v>
+      </c>
+      <c r="C16" s="22"/>
       <c r="D16" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="20" t="s">
@@ -1078,7 +1069,7 @@
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C18" s="22"/>
       <c r="D18" s="20" t="s">
@@ -1086,48 +1077,48 @@
       </c>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="22"/>
+      <c r="B19" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="37"/>
       <c r="D19" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
-      <c r="B20" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="37"/>
+    <row r="20" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B20" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="38"/>
       <c r="D20" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B21" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B22" s="29"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="31"/>
-      <c r="F22" s="24"/>
-    </row>
-    <row r="23" spans="2:6" ht="27" thickBot="1">
-      <c r="B23" s="15" t="s">
+      <c r="B21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="31"/>
+      <c r="F21" s="24"/>
+    </row>
+    <row r="22" spans="2:6" ht="27" thickBot="1">
+      <c r="B22" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="20"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="20"/>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="35"/>
+      <c r="D23" s="20" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="24" spans="2:6">
       <c r="B24" s="13" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="C24" s="35"/>
       <c r="D24" s="20" t="s">
@@ -1135,17 +1126,17 @@
       </c>
     </row>
     <row r="25" spans="2:6">
-      <c r="B25" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="35"/>
+      <c r="B25" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="2"/>
       <c r="D25" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26" s="8" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="20" t="s">
@@ -1154,100 +1145,100 @@
     </row>
     <row r="27" spans="2:6">
       <c r="B27" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="C27" s="25"/>
       <c r="D27" s="20" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="25"/>
+        <v>18</v>
+      </c>
+      <c r="C28" s="22"/>
       <c r="D28" s="20" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="25"/>
+        <v>19</v>
+      </c>
+      <c r="C29" s="22"/>
       <c r="D29" s="20" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="22"/>
+        <v>20</v>
+      </c>
+      <c r="C30" s="25"/>
       <c r="D30" s="20" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="22"/>
+        <v>44</v>
+      </c>
+      <c r="C31" s="25"/>
       <c r="D31" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6">
-      <c r="B32" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4">
-      <c r="B33" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B34" s="11"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="21"/>
-    </row>
-    <row r="35" spans="2:4" ht="27" thickBot="1">
-      <c r="B35" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B32" s="11"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="21"/>
+    </row>
+    <row r="33" spans="2:4" ht="27" thickBot="1">
+      <c r="B33" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="20"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="20"/>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="23"/>
+      <c r="D35" s="20" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="36" spans="2:4">
-      <c r="B36" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36" s="14"/>
+      <c r="B36" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="22"/>
       <c r="D36" s="20" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="B37" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" s="23"/>
+        <v>25</v>
+      </c>
+      <c r="C37" s="22"/>
       <c r="D37" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C38" s="22"/>
       <c r="D38" s="20" t="s">
@@ -1256,7 +1247,7 @@
     </row>
     <row r="39" spans="2:4">
       <c r="B39" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C39" s="22"/>
       <c r="D39" s="20" t="s">
@@ -1265,38 +1256,20 @@
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C40" s="22"/>
       <c r="D40" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="2:4">
-      <c r="B41" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" s="22"/>
+    <row r="41" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B41" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="10"/>
       <c r="D41" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4">
-      <c r="B42" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B43" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Getting done with the interpreter
</commit_message>
<xml_diff>
--- a/ROM Progess.xlsx
+++ b/ROM Progess.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
   <si>
     <t>DEMOS</t>
   </si>
@@ -129,9 +129,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Hyper-espace (comme dans Star Wars)</t>
-  </si>
-  <si>
     <t>Problème</t>
   </si>
   <si>
@@ -141,34 +138,28 @@
     <t>Test de son</t>
   </si>
   <si>
-    <t>Unknown opcode</t>
-  </si>
-  <si>
-    <t>Écran blanc en fin de partie</t>
-  </si>
-  <si>
     <t>alien</t>
   </si>
   <si>
-    <t>tetris</t>
-  </si>
-  <si>
-    <t>Écran rouge après 1ère mort</t>
-  </si>
-  <si>
     <t>boing</t>
   </si>
   <si>
     <t>xor</t>
   </si>
   <si>
-    <t>MegaManX16</t>
-  </si>
-  <si>
     <t>dots2</t>
   </si>
   <si>
-    <t>Point unique alors qu'on devrait voir une droite</t>
+    <t>Le nouveau dispatch semble avoir ralenti considérablement cette ROM</t>
+  </si>
+  <si>
+    <t>Pacman</t>
+  </si>
+  <si>
+    <t>Jeu de son</t>
+  </si>
+  <si>
+    <t>Point unique alors qu'on devrait voir une ligne</t>
   </si>
 </sst>
 </file>
@@ -584,17 +575,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,18 +880,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:G41"/>
+  <dimension ref="B1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="65.7109375" customWidth="1"/>
-    <col min="5" max="5" width="3.5703125" customWidth="1"/>
+    <col min="4" max="4" width="68.5703125" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -927,7 +918,7 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="15.75" thickBot="1">
@@ -938,10 +929,10 @@
       <c r="D5" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="33"/>
+      <c r="G5" s="38"/>
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="8" t="s">
@@ -971,24 +962,24 @@
     </row>
     <row r="8" spans="2:7">
       <c r="B8" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C8" s="22"/>
       <c r="D8" s="20" t="s">
         <v>36</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" s="28"/>
     </row>
     <row r="9" spans="2:7" ht="15.75" thickBot="1">
       <c r="B9" s="8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>34</v>
@@ -1008,7 +999,7 @@
       <c r="B11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="34"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="20" t="s">
         <v>36</v>
       </c>
@@ -1028,7 +1019,7 @@
       </c>
       <c r="C13" s="22"/>
       <c r="D13" s="20" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="2:7">
@@ -1037,16 +1028,16 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="25"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="2:7">
@@ -1055,7 +1046,7 @@
       </c>
       <c r="C16" s="22"/>
       <c r="D16" s="20" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="2:6">
@@ -1077,19 +1068,19 @@
       </c>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="37"/>
+      <c r="B19" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="35"/>
       <c r="D19" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="15.75" thickBot="1">
       <c r="B20" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="38"/>
+        <v>42</v>
+      </c>
+      <c r="C20" s="36"/>
       <c r="D20" s="20" t="s">
         <v>36</v>
       </c>
@@ -1109,9 +1100,9 @@
     </row>
     <row r="23" spans="2:6">
       <c r="B23" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="35"/>
+        <v>40</v>
+      </c>
+      <c r="C23" s="33"/>
       <c r="D23" s="20" t="s">
         <v>36</v>
       </c>
@@ -1120,7 +1111,7 @@
       <c r="B24" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="35"/>
+      <c r="C24" s="33"/>
       <c r="D24" s="20" t="s">
         <v>36</v>
       </c>
@@ -1131,25 +1122,25 @@
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="20" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="C26" s="22"/>
       <c r="D26" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="25"/>
+        <v>45</v>
+      </c>
+      <c r="C27" s="22"/>
       <c r="D27" s="20" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="2:6">
@@ -1174,53 +1165,53 @@
       <c r="B30" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="25"/>
+      <c r="C30" s="22"/>
       <c r="D30" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6">
-      <c r="B31" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B32" s="11"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="21"/>
-    </row>
-    <row r="33" spans="2:4" ht="27" thickBot="1">
-      <c r="B33" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B31" s="11"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="21"/>
+    </row>
+    <row r="32" spans="2:6" ht="27" thickBot="1">
+      <c r="B32" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="20"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="20"/>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="20" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="34" spans="2:4">
-      <c r="B34" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" s="14"/>
+      <c r="B34" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="23"/>
       <c r="D34" s="20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="23"/>
+        <v>24</v>
+      </c>
+      <c r="C35" s="22"/>
       <c r="D35" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C36" s="22"/>
       <c r="D36" s="20" t="s">
@@ -1229,7 +1220,7 @@
     </row>
     <row r="37" spans="2:4">
       <c r="B37" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C37" s="22"/>
       <c r="D37" s="20" t="s">
@@ -1238,7 +1229,7 @@
     </row>
     <row r="38" spans="2:4">
       <c r="B38" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C38" s="22"/>
       <c r="D38" s="20" t="s">
@@ -1247,29 +1238,20 @@
     </row>
     <row r="39" spans="2:4">
       <c r="B39" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C39" s="22"/>
       <c r="D39" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="2:4">
-      <c r="B40" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="22"/>
+    <row r="40" spans="2:4" ht="15.75" thickBot="1">
+      <c r="B40" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="10"/>
       <c r="D40" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" ht="15.75" thickBot="1">
-      <c r="B41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Starting to see some ROMs working again
</commit_message>
<xml_diff>
--- a/ROM Progess.xlsx
+++ b/ROM Progess.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
   <si>
     <t>DEMOS</t>
   </si>
@@ -150,16 +150,37 @@
     <t>dots2</t>
   </si>
   <si>
-    <t>Le nouveau dispatch semble avoir ralenti considérablement cette ROM</t>
-  </si>
-  <si>
     <t>Pacman</t>
   </si>
   <si>
     <t>Jeu de son</t>
   </si>
   <si>
-    <t>Point unique alors qu'on devrait voir une ligne</t>
+    <t>Écran blanc</t>
+  </si>
+  <si>
+    <t>Pas de détection de collisions</t>
+  </si>
+  <si>
+    <t>Sketchy…</t>
+  </si>
+  <si>
+    <t>Texte disparaît</t>
+  </si>
+  <si>
+    <t>Démo de son</t>
+  </si>
+  <si>
+    <t>Un seul point statique</t>
+  </si>
+  <si>
+    <t>Semble un peu lent</t>
+  </si>
+  <si>
+    <t>Écran noir</t>
+  </si>
+  <si>
+    <t>Non borné en bas et à droite</t>
   </si>
 </sst>
 </file>
@@ -532,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -576,7 +597,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -882,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -929,10 +949,10 @@
       <c r="D5" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="38"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="8" t="s">
@@ -951,9 +971,9 @@
       <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="20" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>33</v>
@@ -979,7 +999,7 @@
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>34</v>
@@ -990,9 +1010,9 @@
       <c r="B10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="20" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="2:7">
@@ -1008,18 +1028,18 @@
       <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="22"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="20" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="2:7">
@@ -1028,16 +1048,16 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="20" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="22"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="20" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="2:7">
@@ -1046,14 +1066,14 @@
       </c>
       <c r="C16" s="22"/>
       <c r="D16" s="20" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="C17" s="2"/>
       <c r="D17" s="20" t="s">
         <v>36</v>
       </c>
@@ -1068,10 +1088,10 @@
       </c>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="35"/>
+      <c r="C19" s="34"/>
       <c r="D19" s="20" t="s">
         <v>36</v>
       </c>
@@ -1080,7 +1100,7 @@
       <c r="B20" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="36"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="20" t="s">
         <v>36</v>
       </c>
@@ -1102,7 +1122,7 @@
       <c r="B23" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="33"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="20" t="s">
         <v>36</v>
       </c>
@@ -1111,7 +1131,7 @@
       <c r="B24" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="33"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="20" t="s">
         <v>36</v>
       </c>
@@ -1122,23 +1142,23 @@
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="22"/>
+      <c r="C26" s="2"/>
       <c r="D26" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="22"/>
+        <v>44</v>
+      </c>
+      <c r="C27" s="2"/>
       <c r="D27" s="20" t="s">
         <v>36</v>
       </c>
@@ -1147,7 +1167,7 @@
       <c r="B28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="22"/>
+      <c r="C28" s="2"/>
       <c r="D28" s="20" t="s">
         <v>36</v>
       </c>
@@ -1156,7 +1176,7 @@
       <c r="B29" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="22"/>
+      <c r="C29" s="2"/>
       <c r="D29" s="20" t="s">
         <v>36</v>
       </c>
@@ -1165,7 +1185,7 @@
       <c r="B30" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="22"/>
+      <c r="C30" s="2"/>
       <c r="D30" s="20" t="s">
         <v>36</v>
       </c>
@@ -1204,9 +1224,9 @@
       <c r="B35" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="22"/>
+      <c r="C35" s="25"/>
       <c r="D35" s="20" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="2:4">

</xml_diff>

<commit_message>
Bugfix + basic block fetching + continue paper review
</commit_message>
<xml_diff>
--- a/ROM Progess.xlsx
+++ b/ROM Progess.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t>DEMOS</t>
   </si>
@@ -156,31 +156,16 @@
     <t>Jeu de son</t>
   </si>
   <si>
-    <t>Écran blanc</t>
-  </si>
-  <si>
-    <t>Pas de détection de collisions</t>
-  </si>
-  <si>
     <t>Sketchy…</t>
   </si>
   <si>
-    <t>Texte disparaît</t>
-  </si>
-  <si>
     <t>Démo de son</t>
   </si>
   <si>
-    <t>Un seul point statique</t>
-  </si>
-  <si>
     <t>Semble un peu lent</t>
   </si>
   <si>
-    <t>Écran noir</t>
-  </si>
-  <si>
-    <t>Non borné en bas et à droite</t>
+    <t>Kunais apparaîssent proches du joueur</t>
   </si>
 </sst>
 </file>
@@ -553,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -606,6 +591,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -902,8 +888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -971,9 +957,9 @@
       <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="25"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="20" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>33</v>
@@ -999,7 +985,7 @@
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>34</v>
@@ -1010,9 +996,9 @@
       <c r="B10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="25"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="20" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="2:7">
@@ -1028,18 +1014,18 @@
       <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="25"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="20" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="25"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="20" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:7">
@@ -1048,16 +1034,16 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="25"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="20" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="2:7">
@@ -1066,7 +1052,7 @@
       </c>
       <c r="C16" s="22"/>
       <c r="D16" s="20" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="2:6">
@@ -1122,7 +1108,7 @@
       <c r="B23" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="14"/>
+      <c r="C23" s="38"/>
       <c r="D23" s="20" t="s">
         <v>36</v>
       </c>
@@ -1131,7 +1117,7 @@
       <c r="B24" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="14"/>
+      <c r="C24" s="38"/>
       <c r="D24" s="20" t="s">
         <v>36</v>
       </c>
@@ -1149,16 +1135,16 @@
       <c r="B26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="25"/>
       <c r="D26" s="20" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="22"/>
       <c r="D27" s="20" t="s">
         <v>36</v>
       </c>
@@ -1167,7 +1153,7 @@
       <c r="B28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="20" t="s">
         <v>36</v>
       </c>
@@ -1176,7 +1162,7 @@
       <c r="B29" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="2"/>
+      <c r="C29" s="22"/>
       <c r="D29" s="20" t="s">
         <v>36</v>
       </c>
@@ -1185,7 +1171,7 @@
       <c r="B30" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30" s="22"/>
       <c r="D30" s="20" t="s">
         <v>36</v>
       </c>
@@ -1224,9 +1210,9 @@
       <c r="B35" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="25"/>
+      <c r="C35" s="22"/>
       <c r="D35" s="20" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="2:4">

</xml_diff>

<commit_message>
Fixing command line interface + fixing flip + article writing
</commit_message>
<xml_diff>
--- a/ROM Progess.xlsx
+++ b/ROM Progess.xlsx
@@ -585,13 +585,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -888,8 +888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -935,10 +935,10 @@
       <c r="D5" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="37"/>
+      <c r="G5" s="38"/>
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="8" t="s">
@@ -1108,7 +1108,7 @@
       <c r="B23" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="38"/>
+      <c r="C23" s="36"/>
       <c r="D23" s="20" t="s">
         <v>36</v>
       </c>
@@ -1117,7 +1117,7 @@
       <c r="B24" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="38"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="20" t="s">
         <v>36</v>
       </c>

</xml_diff>